<commit_message>
added a few potential rift-only monsters
</commit_message>
<xml_diff>
--- a/Graphic changes required.xlsx
+++ b/Graphic changes required.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dip in IT 2012\Year 3\Game Programming\Assignment 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dip in IT 2012\Year 3\Game Programming\Assignment 2\gp-assignment-2-rpg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Image Name</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>Nets are used as the main way to catch fish.</t>
+  </si>
+  <si>
+    <t>Giant Rat</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>Grizzly Bear</t>
   </si>
 </sst>
 </file>
@@ -251,7 +260,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -269,6 +298,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -558,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +661,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -642,7 +681,7 @@
         <v>42</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -662,7 +701,7 @@
         <v>45</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -682,7 +721,7 @@
         <v>48</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -702,7 +741,7 @@
         <v>54</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -722,7 +761,7 @@
         <v>57</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -759,7 +798,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
@@ -779,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -799,7 +838,7 @@
         <v>39</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -819,7 +858,7 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
@@ -839,7 +878,7 @@
         <v>33</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -859,7 +898,7 @@
         <v>24</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
@@ -879,7 +918,7 @@
         <v>36</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
@@ -899,7 +938,7 @@
         <v>51</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
@@ -926,6 +965,48 @@
       </c>
       <c r="E18" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -933,7 +1014,7 @@
   <sortState ref="A2:F18">
     <sortCondition ref="C2"/>
   </sortState>
-  <conditionalFormatting sqref="C2:C18">
+  <conditionalFormatting sqref="C2:C21">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -945,12 +1026,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D18">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="D2:D21">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Graphic changes required file update
</commit_message>
<xml_diff>
--- a/Graphic changes required.xlsx
+++ b/Graphic changes required.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
   <si>
     <t>Image Name</t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t>Grizzly Bear</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>NPC</t>
+  </si>
+  <si>
+    <t>Raid Boss</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Enemy</t>
   </si>
 </sst>
 </file>
@@ -597,424 +615,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="C4">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C9" t="s">
         <v>45</v>
       </c>
-      <c r="C5">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="C6">
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="C7">
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E11" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F11" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C12" t="s">
         <v>57</v>
       </c>
-      <c r="C8">
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
         <v>22</v>
       </c>
-      <c r="F9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="G20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F21" t="s">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
-  <sortState ref="A2:F18">
-    <sortCondition ref="C2"/>
+  <sortState ref="A2:G21">
+    <sortCondition ref="D2"/>
   </sortState>
-  <conditionalFormatting sqref="C2:C21">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1026,12 +1104,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="E2:E21">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",D2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("No",E2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",D2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more planend changes
</commit_message>
<xml_diff>
--- a/Graphic changes required.xlsx
+++ b/Graphic changes required.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="89">
   <si>
     <t>Image Name</t>
   </si>
@@ -237,6 +237,63 @@
   </si>
   <si>
     <t>Enemy</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Quest Screen</t>
+  </si>
+  <si>
+    <t>Talk Screen</t>
+  </si>
+  <si>
+    <t>Dark Realm Overlay</t>
+  </si>
+  <si>
+    <t>assets\ui\windowbackground.png</t>
+  </si>
+  <si>
+    <t>Currently a black image with an alpha of 0.66 is overlaid directly on top of the game.</t>
+  </si>
+  <si>
+    <t>Rift Close Animation</t>
+  </si>
+  <si>
+    <t>Rift Enter Animation</t>
+  </si>
+  <si>
+    <t>Rift Exit Animation</t>
+  </si>
+  <si>
+    <t>Level up skill effect</t>
+  </si>
+  <si>
+    <t>Quest Complete Effect</t>
+  </si>
+  <si>
+    <t>Shop window</t>
+  </si>
+  <si>
+    <t>Played right after rift exit animation</t>
+  </si>
+  <si>
+    <t>Player enters the rift</t>
+  </si>
+  <si>
+    <t>Player exits the rift</t>
+  </si>
+  <si>
+    <t>Played directly on the screen on level up</t>
+  </si>
+  <si>
+    <t>Played directly on the screen on quest complete; note that the quest complete screen will also be shown</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>x32x32</t>
   </si>
 </sst>
 </file>
@@ -278,64 +335,384 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="38">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -615,9 +992,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1086,6 +1465,156 @@
       </c>
       <c r="F21" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1104,11 +1633,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E21">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+  <conditionalFormatting sqref="E2:E30 F22:F30">
+    <cfRule type="containsText" dxfId="37" priority="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="36" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>